<commit_message>
Minor Changes to BOM and Case
</commit_message>
<xml_diff>
--- a/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
+++ b/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="SwitchBoard" localSheetId="0">BOM!$A$1:$I$74</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -559,7 +559,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1134,6 +1134,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1185,7 +1188,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1220,7 +1223,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1432,8 +1435,8 @@
   <dimension ref="A1:I80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B72" sqref="B72"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3351,7 +3354,7 @@
         <v>157</v>
       </c>
       <c r="G74" s="8">
-        <v>2443114</v>
+        <v>2443113</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Minor Silkscreen updates to SwitchBoard. New Gerber files and updated BOM and P&P with lipo connector
</commit_message>
<xml_diff>
--- a/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
+++ b/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
@@ -8,9 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="SwitchBoard" localSheetId="0">BOM!$A$1:$I$74</definedName>
+    <definedName name="SwitchBoard" localSheetId="0">BOM!$A$1:$I$75</definedName>
+    <definedName name="SwitchBoardNew" localSheetId="1">Sheet1!$A$1:$L$88</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -37,11 +39,29 @@
       </textFields>
     </textPr>
   </connection>
+  <connection id="2" name="SwitchBoardNew" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoardNew.csv" tab="0" semicolon="1" consecutive="1">
+      <textFields count="12">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="233">
   <si>
     <t>Part</t>
   </si>
@@ -427,9 +447,6 @@
     <t>PNP Transistror</t>
   </si>
   <si>
-    <t>USB Connectors</t>
-  </si>
-  <si>
     <t>PCB Train Free Component Stock</t>
   </si>
   <si>
@@ -514,9 +531,6 @@
     <t>TPS61090RSARG4</t>
   </si>
   <si>
-    <t>USB3070-30-A</t>
-  </si>
-  <si>
     <t>CAPACITOR, European symbol</t>
   </si>
   <si>
@@ -554,13 +568,205 @@
   </si>
   <si>
     <t>PCBTRAIN FREE</t>
+  </si>
+  <si>
+    <t>47346-0001</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>OC_NEWARK</t>
+  </si>
+  <si>
+    <t>PACKAGE</t>
+  </si>
+  <si>
+    <t>PROD_ID</t>
+  </si>
+  <si>
+    <t>SUPPLIER</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>M02PTH</t>
+  </si>
+  <si>
+    <t>1X02</t>
+  </si>
+  <si>
+    <t>Header 2</t>
+  </si>
+  <si>
+    <t>JP2</t>
+  </si>
+  <si>
+    <t>LiPoIN</t>
+  </si>
+  <si>
+    <t>JP3</t>
+  </si>
+  <si>
+    <t>LiPo</t>
+  </si>
+  <si>
+    <t>M02-JST-2MM-SMT</t>
+  </si>
+  <si>
+    <t>JST-2-SMD</t>
+  </si>
+  <si>
+    <t>JP4</t>
+  </si>
+  <si>
+    <t>PWR</t>
+  </si>
+  <si>
+    <t>PINHD-1X2</t>
+  </si>
+  <si>
+    <t>PIN HEADER</t>
+  </si>
+  <si>
+    <t>JP5</t>
+  </si>
+  <si>
+    <t>Shld</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>JP8</t>
+  </si>
+  <si>
+    <t>CS_IN+</t>
+  </si>
+  <si>
+    <t>PINHD-1X1</t>
+  </si>
+  <si>
+    <t>1X01</t>
+  </si>
+  <si>
+    <t>JP9</t>
+  </si>
+  <si>
+    <t>CS_IN-</t>
+  </si>
+  <si>
+    <t>08P2857</t>
+  </si>
+  <si>
+    <t>Wuerth Elektronik</t>
+  </si>
+  <si>
+    <t>U$1</t>
+  </si>
+  <si>
+    <t>PINHD-3X7GAP</t>
+  </si>
+  <si>
+    <t>3X07</t>
+  </si>
+  <si>
+    <t>IC-09995</t>
+  </si>
+  <si>
+    <t>59K1531</t>
+  </si>
+  <si>
+    <t>TSSOP-24</t>
+  </si>
+  <si>
+    <t>Analog Devices</t>
+  </si>
+  <si>
+    <t>57M6035</t>
+  </si>
+  <si>
+    <t>73T8174</t>
+  </si>
+  <si>
+    <t>16-Lead SOIC_W</t>
+  </si>
+  <si>
+    <t>MOLEX_47346-0001</t>
+  </si>
+  <si>
+    <t>CONN RCPT 5POS MICRO USB R/A  SMD</t>
+  </si>
+  <si>
+    <t>47M0505</t>
+  </si>
+  <si>
+    <t>5 POS MICRO USB R/A</t>
+  </si>
+  <si>
+    <t>MOLEX</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>CTR_ARD</t>
+  </si>
+  <si>
+    <t>F09HP</t>
+  </si>
+  <si>
+    <t>SUB-D</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>CTR_OUT</t>
+  </si>
+  <si>
+    <t>M09HP</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>DSUB _T</t>
+  </si>
+  <si>
+    <t>F37HP</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>DSUB_B</t>
+  </si>
+  <si>
+    <t>M37HP</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>CTR_IN</t>
+  </si>
+  <si>
+    <t> S2B-PH-SM4-TB(LF)(SN)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,13 +918,6 @@
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color rgb="FF3C3C3C"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1063,7 +1262,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1090,7 +1289,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1151,6 +1349,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoard" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoardNew" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1444,7 +1646,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G74" sqref="G74"/>
+      <selection pane="bottomLeft" activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,7 +1656,7 @@
     <col min="3" max="3" width="42.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="9" customWidth="1"/>
     <col min="8" max="8" width="30.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="9" customWidth="1"/>
@@ -1484,7 +1686,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1501,10 +1703,10 @@
         <v>10</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G2" s="4">
         <v>2320852</v>
@@ -1524,10 +1726,10 @@
         <v>10</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G3" s="4">
         <v>2320852</v>
@@ -1547,10 +1749,10 @@
         <v>10</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G4" s="4">
         <v>2320852</v>
@@ -1570,16 +1772,16 @@
         <v>10</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G5" s="5">
         <v>1759265</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -1597,16 +1799,16 @@
         <v>10</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G6" s="5">
         <v>1759265</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -1624,16 +1826,16 @@
         <v>10</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="5">
         <v>1759265</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -1651,16 +1853,16 @@
         <v>10</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G8" s="5">
         <v>1759265</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -1678,16 +1880,16 @@
         <v>10</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G9" s="5">
         <v>1759265</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1705,16 +1907,16 @@
         <v>10</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G10" s="11">
         <v>2320829</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -1732,10 +1934,10 @@
         <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G11" s="7">
         <v>2353063</v>
@@ -1755,10 +1957,10 @@
         <v>10</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G12" s="4">
         <v>2320852</v>
@@ -1778,16 +1980,16 @@
         <v>10</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G13" s="5">
         <v>1759265</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -1805,16 +2007,16 @@
         <v>10</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G14" s="5">
         <v>1759265</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -1832,16 +2034,16 @@
         <v>10</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G15" s="11">
         <v>1759246</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I15" s="2"/>
     </row>
@@ -1859,10 +2061,10 @@
         <v>24</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G16" s="7">
         <v>2353063</v>
@@ -1884,16 +2086,16 @@
         <v>10</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="5">
         <v>1759265</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -1911,16 +2113,16 @@
         <v>10</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G18" s="5">
         <v>1759265</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -1938,16 +2140,16 @@
         <v>10</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G19" s="5">
         <v>1759265</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I19" s="2"/>
     </row>
@@ -1965,16 +2167,16 @@
         <v>10</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G20" s="5">
         <v>2320827</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I20" s="2"/>
     </row>
@@ -1992,16 +2194,16 @@
         <v>10</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G21" s="5">
         <v>1759265</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I21" s="2"/>
     </row>
@@ -2019,16 +2221,16 @@
         <v>10</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G22" s="5">
         <v>2320827</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I22" s="2"/>
     </row>
@@ -2046,16 +2248,16 @@
         <v>10</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G23" s="5">
         <v>1759265</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I23" s="2"/>
     </row>
@@ -2073,16 +2275,16 @@
         <v>10</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G24" s="5">
         <v>1759265</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I24" s="2"/>
     </row>
@@ -2100,16 +2302,16 @@
         <v>10</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G25" s="5">
         <v>1759265</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I25" s="2"/>
     </row>
@@ -2127,16 +2329,16 @@
         <v>10</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G26" s="5">
         <v>2320827</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I26" s="2"/>
     </row>
@@ -2154,16 +2356,16 @@
         <v>10</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G27" s="5">
         <v>1759265</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I27" s="2"/>
     </row>
@@ -2181,76 +2383,72 @@
         <v>10</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G28" s="5">
         <v>2320827</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="G29" s="8">
+        <v>9492615</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B30" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="F29" s="9" t="s">
+      <c r="E30" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G30" s="7">
         <v>1635987</v>
-      </c>
-      <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="G30" s="11">
-        <v>2099243</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>55</v>
@@ -2262,19 +2460,19 @@
         <v>57</v>
       </c>
       <c r="F31" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="G31" s="7">
-        <v>2099235</v>
+        <v>135</v>
+      </c>
+      <c r="G31" s="11">
+        <v>2099243</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B32" s="9" t="s">
         <v>59</v>
@@ -2289,22 +2487,22 @@
         <v>57</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G32" s="7">
         <v>2099235</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>161</v>
+        <v>60</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>55</v>
@@ -2316,49 +2514,49 @@
         <v>57</v>
       </c>
       <c r="F33" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="G33" s="11">
+        <v>133</v>
+      </c>
+      <c r="G33" s="7">
+        <v>2099235</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="2"/>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="G34" s="11">
         <v>2099236</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+      <c r="H34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="I34" s="2"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B34" s="9">
+      <c r="B35" s="9">
         <v>470</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G34" s="5">
-        <v>2129087</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>66</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>63</v>
@@ -2367,25 +2565,25 @@
         <v>64</v>
       </c>
       <c r="E35" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="G35" s="11">
-        <v>2129113</v>
+        <v>160</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="5">
+        <v>2129087</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="9" t="s">
         <v>63</v>
@@ -2394,25 +2592,25 @@
         <v>64</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G36" s="11">
-        <v>2129135</v>
+        <v>2129113</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="9" t="s">
         <v>63</v>
@@ -2421,25 +2619,25 @@
         <v>64</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G37" s="11">
-        <v>2129375</v>
+        <v>2129135</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>63</v>
@@ -2448,25 +2646,25 @@
         <v>64</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G38" s="11">
-        <v>2129319</v>
+        <v>2129375</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>63</v>
@@ -2475,22 +2673,22 @@
         <v>64</v>
       </c>
       <c r="E39" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G39" s="5">
-        <v>9332391</v>
+        <v>160</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G39" s="11">
+        <v>2129319</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>74</v>
@@ -2502,25 +2700,25 @@
         <v>64</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G40" s="5">
         <v>9332391</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>63</v>
@@ -2529,25 +2727,25 @@
         <v>64</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G41" s="11">
-        <v>2129372</v>
+        <v>160</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G41" s="5">
+        <v>9332391</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>63</v>
@@ -2556,25 +2754,25 @@
         <v>64</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="G42" s="11">
-        <v>2351393</v>
+        <v>2129372</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C43" s="9" t="s">
         <v>63</v>
@@ -2583,25 +2781,25 @@
         <v>64</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G43" s="11">
-        <v>2129375</v>
+        <v>2351393</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>63</v>
@@ -2610,25 +2808,25 @@
         <v>64</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="G44" s="11">
-        <v>2129113</v>
+        <v>2129375</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>63</v>
@@ -2637,22 +2835,22 @@
         <v>64</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G45" s="5">
-        <v>9332391</v>
+        <v>160</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" s="11">
+        <v>2129113</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B46" s="9" t="s">
         <v>74</v>
@@ -2664,25 +2862,25 @@
         <v>64</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G46" s="5">
         <v>9332391</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>63</v>
@@ -2691,25 +2889,25 @@
         <v>64</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F47" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="G47" s="11">
-        <v>2129250</v>
+        <v>160</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G47" s="5">
+        <v>9332391</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>63</v>
@@ -2718,25 +2916,25 @@
         <v>64</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F48" s="10" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="G48" s="11">
-        <v>2129329</v>
+        <v>2129250</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>63</v>
@@ -2745,25 +2943,25 @@
         <v>64</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F49" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="G49" s="11">
-        <v>2129113</v>
+        <v>2129329</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>63</v>
@@ -2772,22 +2970,22 @@
         <v>64</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G50" s="5">
-        <v>9332391</v>
+        <v>160</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="G50" s="11">
+        <v>2129113</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B51" s="9" t="s">
         <v>74</v>
@@ -2799,22 +2997,22 @@
         <v>64</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G51" s="5">
         <v>9332391</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B52" s="9" t="s">
         <v>74</v>
@@ -2826,21 +3024,22 @@
         <v>64</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G52" s="5">
         <v>9332391</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>129</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B53" s="9" t="s">
         <v>74</v>
@@ -2852,21 +3051,21 @@
         <v>64</v>
       </c>
       <c r="E53" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G53" s="5">
         <v>9332391</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>74</v>
@@ -2878,21 +3077,21 @@
         <v>64</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G54" s="5">
         <v>9332391</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>74</v>
@@ -2904,24 +3103,24 @@
         <v>64</v>
       </c>
       <c r="E55" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G55" s="5">
         <v>9332391</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>97</v>
+        <v>74</v>
       </c>
       <c r="C56" s="9" t="s">
         <v>63</v>
@@ -2930,21 +3129,21 @@
         <v>64</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="F56" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="G56" s="11">
-        <v>2129417</v>
+        <v>160</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G56" s="5">
+        <v>9332391</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B57" s="9" t="s">
         <v>97</v>
@@ -2956,95 +3155,97 @@
         <v>64</v>
       </c>
       <c r="E57" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F57" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G57" s="11">
         <v>2129417</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G58" s="11">
+        <v>2129417</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B59" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C59" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D59" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E59" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F58" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="G58" s="11">
+      <c r="F59" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="G59" s="11">
         <v>2336778</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B59" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C59" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D59" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="E59" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="F59" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="G59" s="8">
-        <v>1332158</v>
-      </c>
-      <c r="H59" s="2"/>
+      <c r="H59" s="2" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D60" s="9" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E60" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G60" s="9">
-        <v>9604367</v>
+        <v>161</v>
+      </c>
+      <c r="F60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="G60" s="8">
+        <v>1332158</v>
       </c>
       <c r="H60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B61" s="9" t="s">
         <v>107</v>
@@ -3056,7 +3257,7 @@
         <v>108</v>
       </c>
       <c r="E61" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F61" s="7" t="s">
         <v>107</v>
@@ -3068,53 +3269,54 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E62" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G62" s="8">
-        <v>1207334</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="F62" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G62" s="9">
+        <v>9604367</v>
+      </c>
+      <c r="H62" s="2"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="E63" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G63" s="9">
-        <v>9604367</v>
+        <v>163</v>
+      </c>
+      <c r="F63" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G63" s="8">
+        <v>1207334</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>107</v>
@@ -3126,7 +3328,7 @@
         <v>108</v>
       </c>
       <c r="E64" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>107</v>
@@ -3137,7 +3339,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>107</v>
@@ -3149,9 +3351,9 @@
         <v>108</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="F65" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="F65" s="7" t="s">
         <v>107</v>
       </c>
       <c r="G65" s="9">
@@ -3160,53 +3362,53 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="C66" s="9" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>46</v>
+        <v>108</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="F66" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G66" s="8">
-        <v>2115900</v>
+        <v>162</v>
+      </c>
+      <c r="F66" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="G66" s="9">
+        <v>9604367</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="C67" s="9" t="s">
-        <v>107</v>
+        <v>45</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>108</v>
+        <v>46</v>
       </c>
       <c r="E67" s="9" t="s">
         <v>164</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="G67" s="9">
-        <v>9604367</v>
+        <v>45</v>
+      </c>
+      <c r="G67" s="8">
+        <v>2115900</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="9" t="s">
         <v>107</v>
@@ -3218,7 +3420,7 @@
         <v>108</v>
       </c>
       <c r="E68" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F68" s="4" t="s">
         <v>107</v>
@@ -3229,7 +3431,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="9" t="s">
         <v>107</v>
@@ -3241,7 +3443,7 @@
         <v>108</v>
       </c>
       <c r="E69" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F69" s="4" t="s">
         <v>107</v>
@@ -3252,53 +3454,53 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C70" s="9" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="E70" s="9" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="G70" s="9">
-        <v>2067770</v>
+        <v>9604367</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="C71" s="9" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="E71" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="G71" s="9">
-        <v>9604367</v>
+        <v>2067770</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
-        <v>168</v>
+        <v>123</v>
       </c>
       <c r="B72" s="9" t="s">
         <v>107</v>
@@ -3310,7 +3512,7 @@
         <v>108</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>107</v>
@@ -3321,88 +3523,1900 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="C73" s="9" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>126</v>
+        <v>162</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="G73" s="9">
-        <v>2377152</v>
+        <v>9604367</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B74" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G74" s="9">
+        <v>2377152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B75" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="C74" s="9" t="s">
+      <c r="C75" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D74" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="E74" s="9" t="s">
-        <v>128</v>
-      </c>
-      <c r="F74" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="G74" s="12">
-        <v>2293836</v>
+      <c r="D75" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="F75" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="G75" s="8">
+        <v>1568026</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D77" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E77" s="4">
-        <f t="array" ref="E77">SUM(1/COUNTIF(G2:G74,G2:G74))</f>
-        <v>29.000000000000021</v>
+        <f t="array" ref="E77">SUM(1/COUNTIF(G2:G75,G2:G75))</f>
+        <v>30.000000000000021</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D78" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E78" s="4">
-        <f>COUNTIF(H2:H74,"PCB*")</f>
+        <f>COUNTIF(H2:H75,"PCB*")</f>
         <v>50</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D79" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E79" s="4">
-        <f>COUNTBLANK(H2:H74)</f>
-        <v>23</v>
+        <f>COUNTBLANK(H2:H75)</f>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D80" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E80" s="4">
         <f>SUM(E78:E79)</f>
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L88"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J1" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" t="s">
+        <v>173</v>
+      </c>
+      <c r="L1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>175</v>
+      </c>
+      <c r="B29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" t="s">
+        <v>178</v>
+      </c>
+      <c r="E29" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>180</v>
+      </c>
+      <c r="B30" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" t="s">
+        <v>177</v>
+      </c>
+      <c r="D30" t="s">
+        <v>178</v>
+      </c>
+      <c r="E30" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>182</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>184</v>
+      </c>
+      <c r="D31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>186</v>
+      </c>
+      <c r="B32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C32" t="s">
+        <v>188</v>
+      </c>
+      <c r="D32" t="s">
+        <v>178</v>
+      </c>
+      <c r="E32" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>190</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" t="s">
+        <v>188</v>
+      </c>
+      <c r="D33" t="s">
+        <v>178</v>
+      </c>
+      <c r="E33" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" t="s">
+        <v>191</v>
+      </c>
+      <c r="C34" t="s">
+        <v>188</v>
+      </c>
+      <c r="D34" t="s">
+        <v>178</v>
+      </c>
+      <c r="E34" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>193</v>
+      </c>
+      <c r="B35" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" t="s">
+        <v>195</v>
+      </c>
+      <c r="D35" t="s">
+        <v>196</v>
+      </c>
+      <c r="E35" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>197</v>
+      </c>
+      <c r="B36" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" t="s">
+        <v>195</v>
+      </c>
+      <c r="D36" t="s">
+        <v>196</v>
+      </c>
+      <c r="E36" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+      <c r="E37" t="s">
+        <v>158</v>
+      </c>
+      <c r="G37">
+        <v>7447779006</v>
+      </c>
+      <c r="H37">
+        <v>1635987</v>
+      </c>
+      <c r="I37" t="s">
+        <v>199</v>
+      </c>
+      <c r="J37">
+        <v>7345</v>
+      </c>
+      <c r="L37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+      <c r="B40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42">
+        <v>470</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D47" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>75</v>
+      </c>
+      <c r="B48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" t="s">
+        <v>64</v>
+      </c>
+      <c r="E48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" t="s">
+        <v>77</v>
+      </c>
+      <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+      <c r="D50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D51" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B52" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" t="s">
+        <v>63</v>
+      </c>
+      <c r="D52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E52" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B53" t="s">
+        <v>74</v>
+      </c>
+      <c r="C53" t="s">
+        <v>63</v>
+      </c>
+      <c r="D53" t="s">
+        <v>64</v>
+      </c>
+      <c r="E53" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" t="s">
+        <v>74</v>
+      </c>
+      <c r="C54" t="s">
+        <v>63</v>
+      </c>
+      <c r="D54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" t="s">
+        <v>63</v>
+      </c>
+      <c r="D55" t="s">
+        <v>64</v>
+      </c>
+      <c r="E55" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
+      </c>
+      <c r="D56" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>66</v>
+      </c>
+      <c r="C57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D57" t="s">
+        <v>64</v>
+      </c>
+      <c r="E57" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" t="s">
+        <v>74</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" t="s">
+        <v>64</v>
+      </c>
+      <c r="E58" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>91</v>
+      </c>
+      <c r="B59" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
+        <v>63</v>
+      </c>
+      <c r="D59" t="s">
+        <v>64</v>
+      </c>
+      <c r="E59" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>92</v>
+      </c>
+      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" t="s">
+        <v>63</v>
+      </c>
+      <c r="D60" t="s">
+        <v>64</v>
+      </c>
+      <c r="E60" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>93</v>
+      </c>
+      <c r="B61" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" t="s">
+        <v>63</v>
+      </c>
+      <c r="D61" t="s">
+        <v>64</v>
+      </c>
+      <c r="E61" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C62" t="s">
+        <v>63</v>
+      </c>
+      <c r="D62" t="s">
+        <v>64</v>
+      </c>
+      <c r="E62" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B63" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" t="s">
+        <v>64</v>
+      </c>
+      <c r="E63" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E64" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>98</v>
+      </c>
+      <c r="B65" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" t="s">
+        <v>63</v>
+      </c>
+      <c r="D65" t="s">
+        <v>64</v>
+      </c>
+      <c r="E65" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" t="s">
+        <v>100</v>
+      </c>
+      <c r="C66" t="s">
+        <v>101</v>
+      </c>
+      <c r="D66" t="s">
+        <v>102</v>
+      </c>
+      <c r="E66" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" t="s">
+        <v>202</v>
+      </c>
+      <c r="C67" t="s">
+        <v>202</v>
+      </c>
+      <c r="D67" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>103</v>
+      </c>
+      <c r="B68" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" t="s">
+        <v>104</v>
+      </c>
+      <c r="D68" t="s">
+        <v>105</v>
+      </c>
+      <c r="E68" t="s">
+        <v>161</v>
+      </c>
+      <c r="K68" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" t="s">
+        <v>107</v>
+      </c>
+      <c r="C69" t="s">
+        <v>107</v>
+      </c>
+      <c r="D69" t="s">
+        <v>108</v>
+      </c>
+      <c r="E69" t="s">
+        <v>162</v>
+      </c>
+      <c r="G69" t="s">
+        <v>107</v>
+      </c>
+      <c r="H69">
+        <v>9604367</v>
+      </c>
+      <c r="I69" t="s">
+        <v>205</v>
+      </c>
+      <c r="J69" t="s">
+        <v>206</v>
+      </c>
+      <c r="L69" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>109</v>
+      </c>
+      <c r="B70" t="s">
+        <v>107</v>
+      </c>
+      <c r="C70" t="s">
+        <v>107</v>
+      </c>
+      <c r="D70" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" t="s">
+        <v>162</v>
+      </c>
+      <c r="G70" t="s">
+        <v>107</v>
+      </c>
+      <c r="H70">
+        <v>9604367</v>
+      </c>
+      <c r="I70" t="s">
+        <v>205</v>
+      </c>
+      <c r="J70" t="s">
+        <v>206</v>
+      </c>
+      <c r="L70" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>110</v>
+      </c>
+      <c r="B71" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" t="s">
+        <v>107</v>
+      </c>
+      <c r="C72" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" t="s">
+        <v>108</v>
+      </c>
+      <c r="E72" t="s">
+        <v>162</v>
+      </c>
+      <c r="G72" t="s">
+        <v>107</v>
+      </c>
+      <c r="H72">
+        <v>9604367</v>
+      </c>
+      <c r="I72" t="s">
+        <v>205</v>
+      </c>
+      <c r="J72" t="s">
+        <v>206</v>
+      </c>
+      <c r="L72" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" t="s">
+        <v>107</v>
+      </c>
+      <c r="C73" t="s">
+        <v>107</v>
+      </c>
+      <c r="D73" t="s">
+        <v>108</v>
+      </c>
+      <c r="E73" t="s">
+        <v>162</v>
+      </c>
+      <c r="G73" t="s">
+        <v>107</v>
+      </c>
+      <c r="H73">
+        <v>9604367</v>
+      </c>
+      <c r="I73" t="s">
+        <v>205</v>
+      </c>
+      <c r="J73" t="s">
+        <v>206</v>
+      </c>
+      <c r="L73" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" t="s">
+        <v>107</v>
+      </c>
+      <c r="C74" t="s">
+        <v>107</v>
+      </c>
+      <c r="D74" t="s">
+        <v>108</v>
+      </c>
+      <c r="E74" t="s">
+        <v>162</v>
+      </c>
+      <c r="G74" t="s">
+        <v>107</v>
+      </c>
+      <c r="H74">
+        <v>9604367</v>
+      </c>
+      <c r="I74" t="s">
+        <v>205</v>
+      </c>
+      <c r="J74" t="s">
+        <v>206</v>
+      </c>
+      <c r="L74" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>117</v>
+      </c>
+      <c r="B75" t="s">
+        <v>45</v>
+      </c>
+      <c r="C75" t="s">
+        <v>45</v>
+      </c>
+      <c r="D75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E75" t="s">
+        <v>164</v>
+      </c>
+      <c r="G75" t="s">
+        <v>45</v>
+      </c>
+      <c r="H75">
+        <v>1556468</v>
+      </c>
+      <c r="I75" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" t="s">
+        <v>107</v>
+      </c>
+      <c r="C76" t="s">
+        <v>107</v>
+      </c>
+      <c r="D76" t="s">
+        <v>108</v>
+      </c>
+      <c r="E76" t="s">
+        <v>162</v>
+      </c>
+      <c r="G76" t="s">
+        <v>107</v>
+      </c>
+      <c r="H76">
+        <v>9604367</v>
+      </c>
+      <c r="I76" t="s">
+        <v>205</v>
+      </c>
+      <c r="J76" t="s">
+        <v>206</v>
+      </c>
+      <c r="L76" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" t="s">
+        <v>107</v>
+      </c>
+      <c r="C77" t="s">
+        <v>107</v>
+      </c>
+      <c r="D77" t="s">
+        <v>108</v>
+      </c>
+      <c r="E77" t="s">
+        <v>162</v>
+      </c>
+      <c r="G77" t="s">
+        <v>107</v>
+      </c>
+      <c r="H77">
+        <v>9604367</v>
+      </c>
+      <c r="I77" t="s">
+        <v>205</v>
+      </c>
+      <c r="J77" t="s">
+        <v>206</v>
+      </c>
+      <c r="L77" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>120</v>
+      </c>
+      <c r="B78" t="s">
+        <v>107</v>
+      </c>
+      <c r="C78" t="s">
+        <v>107</v>
+      </c>
+      <c r="D78" t="s">
+        <v>108</v>
+      </c>
+      <c r="E78" t="s">
+        <v>162</v>
+      </c>
+      <c r="G78" t="s">
+        <v>107</v>
+      </c>
+      <c r="H78">
+        <v>9604367</v>
+      </c>
+      <c r="I78" t="s">
+        <v>205</v>
+      </c>
+      <c r="J78" t="s">
+        <v>206</v>
+      </c>
+      <c r="L78" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>122</v>
+      </c>
+      <c r="B79" t="s">
+        <v>121</v>
+      </c>
+      <c r="C79" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" t="s">
+        <v>48</v>
+      </c>
+      <c r="E79" t="s">
+        <v>165</v>
+      </c>
+      <c r="G79" t="s">
+        <v>121</v>
+      </c>
+      <c r="H79">
+        <v>2067770</v>
+      </c>
+      <c r="I79" t="s">
+        <v>209</v>
+      </c>
+      <c r="J79" t="s">
+        <v>210</v>
+      </c>
+      <c r="L79" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" t="s">
+        <v>107</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" t="s">
+        <v>108</v>
+      </c>
+      <c r="E80" t="s">
+        <v>162</v>
+      </c>
+      <c r="G80" t="s">
+        <v>107</v>
+      </c>
+      <c r="H80">
+        <v>9604367</v>
+      </c>
+      <c r="I80" t="s">
+        <v>205</v>
+      </c>
+      <c r="J80" t="s">
+        <v>206</v>
+      </c>
+      <c r="L80" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>166</v>
+      </c>
+      <c r="B81" t="s">
+        <v>107</v>
+      </c>
+      <c r="C81" t="s">
+        <v>107</v>
+      </c>
+      <c r="D81" t="s">
+        <v>108</v>
+      </c>
+      <c r="E81" t="s">
+        <v>162</v>
+      </c>
+      <c r="G81" t="s">
+        <v>107</v>
+      </c>
+      <c r="H81">
+        <v>9604367</v>
+      </c>
+      <c r="I81" t="s">
+        <v>205</v>
+      </c>
+      <c r="J81" t="s">
+        <v>206</v>
+      </c>
+      <c r="L81" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>167</v>
+      </c>
+      <c r="B82" t="s">
+        <v>47</v>
+      </c>
+      <c r="C82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" t="s">
+        <v>47</v>
+      </c>
+      <c r="H82">
+        <v>2377152</v>
+      </c>
+      <c r="J82" t="s">
+        <v>210</v>
+      </c>
+      <c r="L82" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>124</v>
+      </c>
+      <c r="C83" t="s">
+        <v>169</v>
+      </c>
+      <c r="D83" t="s">
+        <v>211</v>
+      </c>
+      <c r="E83" t="s">
+        <v>212</v>
+      </c>
+      <c r="G83" t="s">
+        <v>169</v>
+      </c>
+      <c r="H83">
+        <v>1568026</v>
+      </c>
+      <c r="I83" t="s">
+        <v>213</v>
+      </c>
+      <c r="J83" t="s">
+        <v>214</v>
+      </c>
+      <c r="L83" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>216</v>
+      </c>
+      <c r="B84" t="s">
+        <v>217</v>
+      </c>
+      <c r="C84" t="s">
+        <v>218</v>
+      </c>
+      <c r="D84" t="s">
+        <v>218</v>
+      </c>
+      <c r="E84" t="s">
+        <v>219</v>
+      </c>
+      <c r="H84" t="s">
+        <v>220</v>
+      </c>
+      <c r="I84" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>221</v>
+      </c>
+      <c r="B85" t="s">
+        <v>222</v>
+      </c>
+      <c r="C85" t="s">
+        <v>223</v>
+      </c>
+      <c r="D85" t="s">
+        <v>223</v>
+      </c>
+      <c r="E85" t="s">
+        <v>219</v>
+      </c>
+      <c r="H85" t="s">
+        <v>220</v>
+      </c>
+      <c r="I85" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>224</v>
+      </c>
+      <c r="B86" t="s">
+        <v>225</v>
+      </c>
+      <c r="C86" t="s">
+        <v>226</v>
+      </c>
+      <c r="D86" t="s">
+        <v>226</v>
+      </c>
+      <c r="E86" t="s">
+        <v>219</v>
+      </c>
+      <c r="H86" t="s">
+        <v>220</v>
+      </c>
+      <c r="I86" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>227</v>
+      </c>
+      <c r="B87" t="s">
+        <v>228</v>
+      </c>
+      <c r="C87" t="s">
+        <v>229</v>
+      </c>
+      <c r="D87" t="s">
+        <v>229</v>
+      </c>
+      <c r="E87" t="s">
+        <v>219</v>
+      </c>
+      <c r="H87" t="s">
+        <v>220</v>
+      </c>
+      <c r="I87" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>230</v>
+      </c>
+      <c r="B88" t="s">
+        <v>231</v>
+      </c>
+      <c r="C88" t="s">
+        <v>218</v>
+      </c>
+      <c r="D88" t="s">
+        <v>218</v>
+      </c>
+      <c r="E88" t="s">
+        <v>219</v>
+      </c>
+      <c r="H88" t="s">
+        <v>220</v>
+      </c>
+      <c r="I88" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated BOM to reflect correct R10, thanks to weilong
</commit_message>
<xml_diff>
--- a/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
+++ b/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="236">
   <si>
     <t>Part</t>
   </si>
@@ -766,6 +766,9 @@
   </si>
   <si>
     <t>cnt non free</t>
+  </si>
+  <si>
+    <t>MC01W08051200K</t>
   </si>
 </sst>
 </file>
@@ -1665,9 +1668,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2387,7 +2390,7 @@
       <c r="I21" s="2"/>
       <c r="J21" s="12">
         <f t="array" ref="J21">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J20, $G$2:$G$75), 0))</f>
-        <v>2129250</v>
+        <v>2129299</v>
       </c>
       <c r="K21" s="9">
         <f t="shared" si="0"/>
@@ -2422,7 +2425,7 @@
       <c r="I22" s="2"/>
       <c r="J22" s="12">
         <f t="array" ref="J22">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J21, $G$2:$G$75), 0))</f>
-        <v>2129329</v>
+        <v>2129250</v>
       </c>
       <c r="K22" s="9">
         <f t="shared" si="0"/>
@@ -2457,7 +2460,7 @@
       <c r="I23" s="2"/>
       <c r="J23" s="12">
         <f t="array" ref="J23">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J22, $G$2:$G$75), 0))</f>
-        <v>2129417</v>
+        <v>2129329</v>
       </c>
       <c r="K23" s="9">
         <f t="shared" si="0"/>
@@ -2492,7 +2495,7 @@
       <c r="I24" s="2"/>
       <c r="J24" s="12">
         <f t="array" ref="J24">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J23, $G$2:$G$75), 0))</f>
-        <v>2336778</v>
+        <v>2129417</v>
       </c>
       <c r="K24" s="9">
         <f t="shared" si="0"/>
@@ -2527,11 +2530,11 @@
       <c r="I25" s="2"/>
       <c r="J25" s="12">
         <f t="array" ref="J25">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J24, $G$2:$G$75), 0))</f>
-        <v>1332158</v>
+        <v>2336778</v>
       </c>
       <c r="K25" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -2562,11 +2565,11 @@
       <c r="I26" s="2"/>
       <c r="J26" s="12">
         <f t="array" ref="J26">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J25, $G$2:$G$75), 0))</f>
-        <v>9604367</v>
+        <v>1332158</v>
       </c>
       <c r="K26" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -2597,11 +2600,11 @@
       <c r="I27" s="2"/>
       <c r="J27" s="12">
         <f t="array" ref="J27">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J26, $G$2:$G$75), 0))</f>
-        <v>1207334</v>
+        <v>9604367</v>
       </c>
       <c r="K27" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -2632,7 +2635,7 @@
       <c r="I28" s="2"/>
       <c r="J28" s="12">
         <f t="array" ref="J28">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J27, $G$2:$G$75), 0))</f>
-        <v>2115900</v>
+        <v>1207334</v>
       </c>
       <c r="K28" s="9">
         <f t="shared" si="0"/>
@@ -2663,7 +2666,7 @@
       </c>
       <c r="J29" s="12">
         <f t="array" ref="J29">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J28, $G$2:$G$75), 0))</f>
-        <v>2067770</v>
+        <v>2115900</v>
       </c>
       <c r="K29" s="9">
         <f t="shared" si="0"/>
@@ -2695,7 +2698,7 @@
       <c r="I30" s="2"/>
       <c r="J30" s="12">
         <f t="array" ref="J30">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J29, $G$2:$G$75), 0))</f>
-        <v>2377152</v>
+        <v>2067770</v>
       </c>
       <c r="K30" s="9">
         <f t="shared" si="0"/>
@@ -2730,7 +2733,7 @@
       <c r="I31" s="2"/>
       <c r="J31" s="12">
         <f t="array" ref="J31">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J30, $G$2:$G$75), 0))</f>
-        <v>1568026</v>
+        <v>2377152</v>
       </c>
       <c r="K31" s="9">
         <f t="shared" si="0"/>
@@ -2763,9 +2766,9 @@
         <v>128</v>
       </c>
       <c r="I32" s="2"/>
-      <c r="J32" s="12" t="e">
+      <c r="J32" s="12">
         <f t="array" ref="J32">INDEX($G$2:$G$75, MATCH(0, COUNTIF($J$1:J31, $G$2:$G$75), 0))</f>
-        <v>#N/A</v>
+        <v>1568026</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -3126,10 +3129,10 @@
         <v>160</v>
       </c>
       <c r="F44" s="10" t="s">
-        <v>150</v>
+        <v>235</v>
       </c>
       <c r="G44" s="11">
-        <v>2129375</v>
+        <v>2129299</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>128</v>
@@ -3935,7 +3938,7 @@
       </c>
       <c r="E77" s="4">
         <f t="array" ref="E77">SUM(1/COUNTIF(G2:G75,G2:G75))</f>
-        <v>30.000000000000021</v>
+        <v>31.000000000000021</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fixed error in BOM
</commit_message>
<xml_diff>
--- a/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
+++ b/src/schematics/ScouseTom_SwitchNetwork/Gerber/SwitchBoard_BOM.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F3E9CB-2773-4F78-B65E-67EEB0194E98}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
@@ -14,13 +15,21 @@
     <definedName name="SwitchBoardNew" localSheetId="1">'BOM2018'!$A$1:$L$95</definedName>
     <definedName name="SwitchBoardNew" localSheetId="0">Sheet1!$A$1:$L$88</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="SwitchBoardNew" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="SwitchBoardNew" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Jimbles\Copy\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoardNew.csv" tab="0" semicolon="1" consecutive="1">
       <textFields count="12">
         <textField/>
@@ -38,7 +47,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="SwitchBoardNew1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="SwitchBoardNew1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\Jimbles\ScouseTom\src\schematics\ScouseTom_SwitchNetwork\Gerber\SwitchBoardNew.csv" tab="0" semicolon="1" consecutive="1">
       <textFields count="13">
         <textField/>
@@ -61,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1121" uniqueCount="257">
   <si>
     <t>Part</t>
   </si>
@@ -829,13 +838,22 @@
   </si>
   <si>
     <t>R38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LT1763CDE-F#PBF </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="22" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -994,6 +1012,22 @@
       <color rgb="FF222426"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1293,7 +1327,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1336,36 +1370,39 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="49">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1393,18 +1430,25 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="43" builtinId="6"/>
+    <cellStyle name="Currency" xfId="44" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="45" builtinId="7"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="46" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1429,11 +1473,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoardNew" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="SwitchBoardNew" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SwitchBoardNew" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="SwitchBoardNew" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1512,6 +1556,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1547,6 +1608,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1722,7 +1800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3511,12 +3589,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G23" sqref="G23:G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F82" sqref="F82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3530,7 +3608,6 @@
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="8"/>
     <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3588,12 +3665,11 @@
       <c r="G2" s="4">
         <v>2320852</v>
       </c>
-      <c r="H2" s="8"/>
-      <c r="J2" s="11">
+      <c r="J2" s="9">
         <f t="array" ref="J2">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J1, $G$2:$G$90), 0))</f>
         <v>2320852</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2">
         <f>COUNTIFS($G$2:$G$90,J2,$H$2:$H$90,"")</f>
         <v>4</v>
       </c>
@@ -3620,12 +3696,11 @@
       <c r="G3" s="4">
         <v>2320852</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <f t="array" ref="J3">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J2, $G$2:$G$90), 0))</f>
         <v>1759265</v>
       </c>
-      <c r="K3" s="8">
+      <c r="K3">
         <f t="shared" ref="K3:K50" si="0">COUNTIFS($G$2:$G$90,J3,$H$2:$H$90,"")</f>
         <v>0</v>
       </c>
@@ -3652,12 +3727,11 @@
       <c r="G4" s="4">
         <v>2320852</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <f t="array" ref="J4">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J3, $G$2:$G$90), 0))</f>
         <v>2320829</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3687,11 +3761,11 @@
       <c r="H5" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <f t="array" ref="J5">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J4, $G$2:$G$90), 0))</f>
         <v>2353063</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -3721,11 +3795,11 @@
       <c r="H6" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <f t="array" ref="J6">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J5, $G$2:$G$90), 0))</f>
         <v>1759246</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3755,11 +3829,11 @@
       <c r="H7" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J7" s="11">
+      <c r="J7" s="9">
         <f t="array" ref="J7">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J6, $G$2:$G$90), 0))</f>
         <v>2320827</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3789,11 +3863,11 @@
       <c r="H8" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J8" s="11">
+      <c r="J8" s="9">
         <f t="array" ref="J8">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J7, $G$2:$G$90), 0))</f>
         <v>1776392</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3823,11 +3897,11 @@
       <c r="H9" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="9">
         <f t="array" ref="J9">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J8, $G$2:$G$90), 0))</f>
         <v>1635987</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -3848,20 +3922,20 @@
       <c r="E10" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <v>2320829</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J10" s="11">
+      <c r="J10" s="9">
         <f t="array" ref="J10">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J9, $G$2:$G$90), 0))</f>
         <v>2099243</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3882,18 +3956,17 @@
       <c r="E11" t="s">
         <v>156</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" t="s">
         <v>140</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="4">
         <v>2353063</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="J11" s="11">
+      <c r="J11" s="9">
         <f t="array" ref="J11">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J10, $G$2:$G$90), 0))</f>
         <v>2099235</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3920,12 +3993,11 @@
       <c r="G12" s="4">
         <v>2320852</v>
       </c>
-      <c r="H12" s="8"/>
-      <c r="J12" s="11">
+      <c r="J12" s="9">
         <f t="array" ref="J12">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J11, $G$2:$G$90), 0))</f>
         <v>2099236</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3955,11 +4027,11 @@
       <c r="H13" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J13" s="11">
+      <c r="J13" s="9">
         <f t="array" ref="J13">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J12, $G$2:$G$90), 0))</f>
         <v>2129087</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -3989,11 +4061,11 @@
       <c r="H14" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="9">
         <f t="array" ref="J14">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J13, $G$2:$G$90), 0))</f>
         <v>2129113</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4014,20 +4086,20 @@
       <c r="E15" t="s">
         <v>155</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15" s="8">
         <v>1759246</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J15" s="11">
+      <c r="J15" s="9">
         <f t="array" ref="J15">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J14, $G$2:$G$90), 0))</f>
         <v>2129135</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4048,18 +4120,18 @@
       <c r="E16" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" t="s">
         <v>140</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="4">
         <v>2353063</v>
       </c>
       <c r="H16" s="2"/>
-      <c r="J16" s="11">
+      <c r="J16" s="9">
         <f t="array" ref="J16">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J15, $G$2:$G$90), 0))</f>
         <v>2129375</v>
       </c>
-      <c r="K16" s="8">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4089,11 +4161,11 @@
       <c r="H17" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="9">
         <f t="array" ref="J17">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J16, $G$2:$G$90), 0))</f>
         <v>2129319</v>
       </c>
-      <c r="K17" s="8">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4123,11 +4195,11 @@
       <c r="H18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="9">
         <f t="array" ref="J18">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J17, $G$2:$G$90), 0))</f>
         <v>9332391</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4157,11 +4229,11 @@
       <c r="H19" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="9">
         <f t="array" ref="J19">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J18, $G$2:$G$90), 0))</f>
         <v>2129372</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4191,11 +4263,11 @@
       <c r="H20" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J20" s="11">
+      <c r="J20" s="9">
         <f t="array" ref="J20">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J19, $G$2:$G$90), 0))</f>
         <v>2351393</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4225,11 +4297,11 @@
       <c r="H21" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J21" s="11">
+      <c r="J21" s="9">
         <f t="array" ref="J21">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J20, $G$2:$G$90), 0))</f>
         <v>2129299</v>
       </c>
-      <c r="K21" s="8">
+      <c r="K21">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4259,11 +4331,11 @@
       <c r="H22" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J22" s="11">
+      <c r="J22" s="9">
         <f t="array" ref="J22">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J21, $G$2:$G$90), 0))</f>
         <v>2129250</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4293,11 +4365,11 @@
       <c r="H23" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J23" s="11">
+      <c r="J23" s="9">
         <f t="array" ref="J23">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J22, $G$2:$G$90), 0))</f>
         <v>2129329</v>
       </c>
-      <c r="K23" s="8">
+      <c r="K23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4327,11 +4399,11 @@
       <c r="H24" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J24" s="11">
+      <c r="J24" s="9">
         <f t="array" ref="J24">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J23, $G$2:$G$90), 0))</f>
         <v>2129417</v>
       </c>
-      <c r="K24" s="8">
+      <c r="K24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4361,11 +4433,11 @@
       <c r="H25" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J25" s="11">
+      <c r="J25" s="9">
         <f t="array" ref="J25">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J24, $G$2:$G$90), 0))</f>
         <v>2336778</v>
       </c>
-      <c r="K25" s="8">
+      <c r="K25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4395,11 +4467,11 @@
       <c r="H26" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J26" s="11">
+      <c r="J26" s="9">
         <f t="array" ref="J26">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J25, $G$2:$G$90), 0))</f>
         <v>1332158</v>
       </c>
-      <c r="K26" s="8">
+      <c r="K26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4429,11 +4501,11 @@
       <c r="H27" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J27" s="11">
+      <c r="J27" s="9">
         <f t="array" ref="J27">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J26, $G$2:$G$90), 0))</f>
         <v>9604367</v>
       </c>
-      <c r="K27" s="8">
+      <c r="K27">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -4463,11 +4535,11 @@
       <c r="H28" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J28" s="11">
+      <c r="J28" s="9">
         <f t="array" ref="J28">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J27, $G$2:$G$90), 0))</f>
         <v>1207334</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4497,11 +4569,11 @@
       <c r="H29" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J29" s="11">
+      <c r="J29" s="9">
         <f t="array" ref="J29">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J28, $G$2:$G$90), 0))</f>
         <v>2115900</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4531,11 +4603,11 @@
       <c r="H30" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J30" s="11">
+      <c r="J30" s="9">
         <f t="array" ref="J30">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J29, $G$2:$G$90), 0))</f>
         <v>2067770</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4562,11 +4634,11 @@
       <c r="G31">
         <v>1635987</v>
       </c>
-      <c r="J31" s="11">
+      <c r="J31" s="9">
         <f t="array" ref="J31">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J30, $G$2:$G$90), 0))</f>
         <v>2377152</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4587,20 +4659,20 @@
       <c r="E32" t="s">
         <v>57</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="G32" s="10">
+      <c r="G32" s="8">
         <v>2099243</v>
       </c>
       <c r="H32" t="s">
         <v>127</v>
       </c>
-      <c r="J32" s="11">
+      <c r="J32" s="9">
         <f t="array" ref="J32">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J31, $G$2:$G$90), 0))</f>
         <v>1568026</v>
       </c>
-      <c r="K32" s="8">
+      <c r="K32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -4621,20 +4693,20 @@
       <c r="E33" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="4">
         <v>2099235</v>
       </c>
-      <c r="H33" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J33" s="11" t="e">
+      <c r="H33" t="s">
+        <v>127</v>
+      </c>
+      <c r="J33" s="9" t="e">
         <f t="array" ref="J33">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J32, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K33" s="8">
+      <c r="K33">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4655,20 +4727,20 @@
       <c r="E34" t="s">
         <v>57</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="4">
         <v>2099235</v>
       </c>
-      <c r="H34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J34" s="11" t="e">
+      <c r="H34" t="s">
+        <v>127</v>
+      </c>
+      <c r="J34" s="9" t="e">
         <f t="array" ref="J34">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J33, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K34" s="8">
+      <c r="K34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4689,20 +4761,20 @@
       <c r="E35" t="s">
         <v>57</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="G35" s="10">
+      <c r="G35" s="8">
         <v>2099236</v>
       </c>
-      <c r="H35" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="J35" s="11" t="e">
+      <c r="H35" t="s">
+        <v>127</v>
+      </c>
+      <c r="J35" s="9" t="e">
         <f t="array" ref="J35">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J34, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K35" s="8">
+      <c r="K35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4732,11 +4804,11 @@
       <c r="H36" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J36" s="11" t="e">
+      <c r="J36" s="9" t="e">
         <f t="array" ref="J36">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J35, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K36" s="8">
+      <c r="K36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4757,20 +4829,20 @@
       <c r="E37" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="9" t="s">
+      <c r="F37" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G37" s="10">
+      <c r="G37" s="8">
         <v>2129113</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J37" s="11" t="e">
+      <c r="J37" s="9" t="e">
         <f t="array" ref="J37">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J36, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K37" s="8">
+      <c r="K37">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4791,20 +4863,20 @@
       <c r="E38" t="s">
         <v>159</v>
       </c>
-      <c r="F38" s="9" t="s">
+      <c r="F38" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="G38" s="10">
+      <c r="G38" s="8">
         <v>2129135</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J38" s="11" t="e">
+      <c r="J38" s="9" t="e">
         <f t="array" ref="J38">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J37, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K38" s="8">
+      <c r="K38">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4825,20 +4897,20 @@
       <c r="E39" t="s">
         <v>159</v>
       </c>
-      <c r="F39" s="9" t="s">
+      <c r="F39" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="8">
         <v>2129375</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J39" s="11" t="e">
+      <c r="J39" s="9" t="e">
         <f t="array" ref="J39">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J38, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K39" s="8">
+      <c r="K39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4859,20 +4931,20 @@
       <c r="E40" t="s">
         <v>159</v>
       </c>
-      <c r="F40" s="9" t="s">
+      <c r="F40" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="8">
         <v>2129319</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J40" s="11" t="e">
+      <c r="J40" s="9" t="e">
         <f t="array" ref="J40">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J39, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K40" s="8">
+      <c r="K40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4902,11 +4974,11 @@
       <c r="H41" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J41" s="11" t="e">
+      <c r="J41" s="9" t="e">
         <f t="array" ref="J41">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J40, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K41" s="8">
+      <c r="K41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4936,11 +5008,11 @@
       <c r="H42" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J42" s="11" t="e">
+      <c r="J42" s="9" t="e">
         <f t="array" ref="J42">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J41, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K42" s="8">
+      <c r="K42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4961,20 +5033,20 @@
       <c r="E43" t="s">
         <v>159</v>
       </c>
-      <c r="F43" s="9" t="s">
+      <c r="F43" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="G43" s="10">
+      <c r="G43" s="8">
         <v>2129372</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J43" s="11" t="e">
+      <c r="J43" s="9" t="e">
         <f t="array" ref="J43">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J42, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K43" s="8">
+      <c r="K43">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -4995,20 +5067,20 @@
       <c r="E44" t="s">
         <v>159</v>
       </c>
-      <c r="F44" s="9" t="s">
+      <c r="F44" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="G44" s="10">
+      <c r="G44" s="8">
         <v>2351393</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J44" s="11" t="e">
+      <c r="J44" s="9" t="e">
         <f t="array" ref="J44">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J43, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K44" s="8">
+      <c r="K44">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5029,20 +5101,20 @@
       <c r="E45" t="s">
         <v>159</v>
       </c>
-      <c r="F45" s="9" t="s">
+      <c r="F45" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="G45" s="10">
+      <c r="G45" s="8">
         <v>2129299</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J45" s="11" t="e">
+      <c r="J45" s="9" t="e">
         <f t="array" ref="J45">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J44, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K45" s="8">
+      <c r="K45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5063,20 +5135,20 @@
       <c r="E46" t="s">
         <v>159</v>
       </c>
-      <c r="F46" s="9" t="s">
+      <c r="F46" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="10">
+      <c r="G46" s="8">
         <v>2129113</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J46" s="11" t="e">
+      <c r="J46" s="9" t="e">
         <f t="array" ref="J46">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J45, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K46" s="8">
+      <c r="K46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5106,11 +5178,11 @@
       <c r="H47" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J47" s="11" t="e">
+      <c r="J47" s="9" t="e">
         <f t="array" ref="J47">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J46, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K47" s="8">
+      <c r="K47">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5140,11 +5212,11 @@
       <c r="H48" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J48" s="11" t="e">
+      <c r="J48" s="9" t="e">
         <f t="array" ref="J48">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J47, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K48" s="8">
+      <c r="K48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5165,20 +5237,20 @@
       <c r="E49" t="s">
         <v>159</v>
       </c>
-      <c r="F49" s="9" t="s">
+      <c r="F49" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="G49" s="10">
+      <c r="G49" s="8">
         <v>2129250</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J49" s="11" t="e">
+      <c r="J49" s="9" t="e">
         <f t="array" ref="J49">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J48, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K49" s="8">
+      <c r="K49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5199,20 +5271,20 @@
       <c r="E50" t="s">
         <v>159</v>
       </c>
-      <c r="F50" s="9" t="s">
+      <c r="F50" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="G50" s="10">
+      <c r="G50" s="8">
         <v>2129329</v>
       </c>
       <c r="H50" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="J50" s="11" t="e">
+      <c r="J50" s="9" t="e">
         <f t="array" ref="J50">INDEX($G$2:$G$90, MATCH(0, COUNTIF($J$1:J49, $G$2:$G$90), 0))</f>
         <v>#N/A</v>
       </c>
-      <c r="K50" s="8">
+      <c r="K50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -5233,10 +5305,10 @@
       <c r="E51" t="s">
         <v>159</v>
       </c>
-      <c r="F51" s="9" t="s">
+      <c r="F51" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="G51" s="10">
+      <c r="G51" s="8">
         <v>2129113</v>
       </c>
       <c r="H51" s="2" t="s">
@@ -5268,7 +5340,7 @@
       <c r="H52" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="K52" s="8">
+      <c r="K52">
         <f>SUM(K2:K50)</f>
         <v>23</v>
       </c>
@@ -5419,10 +5491,10 @@
       <c r="E58" t="s">
         <v>159</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G58" s="10">
+      <c r="G58" s="8">
         <v>2129417</v>
       </c>
       <c r="H58" s="2" t="s">
@@ -5445,10 +5517,10 @@
       <c r="E59" t="s">
         <v>159</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="F59" s="7" t="s">
         <v>152</v>
       </c>
-      <c r="G59" s="10">
+      <c r="G59" s="8">
         <v>2129417</v>
       </c>
       <c r="H59" s="2" t="s">
@@ -5835,10 +5907,10 @@
       <c r="E74" t="s">
         <v>126</v>
       </c>
-      <c r="F74" s="10" t="s">
+      <c r="F74" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="G74" s="10">
+      <c r="G74" s="8">
         <v>2336778</v>
       </c>
       <c r="H74" s="2" t="s">
@@ -5861,10 +5933,10 @@
       <c r="E75" t="s">
         <v>160</v>
       </c>
-      <c r="F75" s="7" t="s">
+      <c r="F75" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G75" s="7">
+      <c r="G75" s="6">
         <v>1332158</v>
       </c>
     </row>
@@ -5884,10 +5956,10 @@
       <c r="E76" t="s">
         <v>161</v>
       </c>
-      <c r="F76" s="6" t="s">
+      <c r="F76" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G76" s="8">
+      <c r="G76">
         <v>9604367</v>
       </c>
     </row>
@@ -5907,10 +5979,10 @@
       <c r="E77" t="s">
         <v>161</v>
       </c>
-      <c r="F77" s="6" t="s">
+      <c r="F77" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G77" s="8">
+      <c r="G77">
         <v>9604367</v>
       </c>
     </row>
@@ -5930,10 +6002,10 @@
       <c r="E78" t="s">
         <v>162</v>
       </c>
-      <c r="F78" s="7" t="s">
+      <c r="F78" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="G78" s="7">
+      <c r="G78" s="6">
         <v>1207334</v>
       </c>
     </row>
@@ -5953,10 +6025,10 @@
       <c r="E79" t="s">
         <v>161</v>
       </c>
-      <c r="F79" s="6" t="s">
+      <c r="F79" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G79" s="8">
+      <c r="G79">
         <v>9604367</v>
       </c>
     </row>
@@ -5976,10 +6048,10 @@
       <c r="E80" t="s">
         <v>161</v>
       </c>
-      <c r="F80" s="6" t="s">
+      <c r="F80" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G80" s="8">
+      <c r="G80">
         <v>9604367</v>
       </c>
     </row>
@@ -5999,10 +6071,10 @@
       <c r="E81" t="s">
         <v>161</v>
       </c>
-      <c r="F81" s="7" t="s">
+      <c r="F81" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G81" s="8">
+      <c r="G81">
         <v>9604367</v>
       </c>
     </row>
@@ -6022,10 +6094,10 @@
       <c r="E82" t="s">
         <v>163</v>
       </c>
-      <c r="F82" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G82" s="7">
+      <c r="F82" t="s">
+        <v>256</v>
+      </c>
+      <c r="G82" s="6">
         <v>2115900</v>
       </c>
     </row>
@@ -6048,7 +6120,7 @@
       <c r="F83" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G83" s="8">
+      <c r="G83">
         <v>9604367</v>
       </c>
     </row>
@@ -6071,7 +6143,7 @@
       <c r="F84" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G84" s="8">
+      <c r="G84">
         <v>9604367</v>
       </c>
     </row>
@@ -6094,7 +6166,7 @@
       <c r="F85" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G85" s="8">
+      <c r="G85">
         <v>9604367</v>
       </c>
     </row>
@@ -6117,7 +6189,7 @@
       <c r="F86" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="G86" s="8">
+      <c r="G86">
         <v>2067770</v>
       </c>
     </row>
@@ -6140,7 +6212,7 @@
       <c r="F87" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G87" s="8">
+      <c r="G87">
         <v>9604367</v>
       </c>
     </row>
@@ -6163,7 +6235,7 @@
       <c r="F88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="G88" s="8">
+      <c r="G88">
         <v>9604367</v>
       </c>
     </row>
@@ -6186,7 +6258,7 @@
       <c r="F89" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G89" s="8">
+      <c r="G89">
         <v>2377152</v>
       </c>
     </row>
@@ -6203,10 +6275,10 @@
       <c r="E90" t="s">
         <v>211</v>
       </c>
-      <c r="F90" s="7" t="s">
+      <c r="F90" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="G90" s="7">
+      <c r="G90" s="6">
         <v>1568026</v>
       </c>
     </row>
@@ -6253,5 +6325,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>